<commit_message>
changed the naming from grade to mark, added commentes, fixed report grammar
</commit_message>
<xml_diff>
--- a/test_files/testGIS.xlsx
+++ b/test_files/testGIS.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Total Att</t>
   </si>
   <si>
-    <t xml:space="preserve">grade</t>
+    <t xml:space="preserve">Mark</t>
   </si>
   <si>
     <t xml:space="preserve">Sejal Saleh A. Alsuhaibani</t>
@@ -1714,10 +1714,10 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.71"/>

</xml_diff>